<commit_message>
Fixed queue delay + uped volumes
</commit_message>
<xml_diff>
--- a/docs/IMR-SampleSubmissionSheet_v10(LASTNAME_MMMDD).xlsx
+++ b/docs/IMR-SampleSubmissionSheet_v10(LASTNAME_MMMDD).xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D8F2DB3-F7A8-4F2D-84A6-63117297086D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ECE3F47-A5F0-46C0-AA4A-68D9C2598115}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="742" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="742" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTIONS (read first)" sheetId="3" r:id="rId1"/>
@@ -15,12 +15,12 @@
     <sheet name="Genome Samples" sheetId="11" r:id="rId5"/>
     <sheet name="Metagenomic Samples" sheetId="9" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179017" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="157">
   <si>
     <t xml:space="preserve">Plate 1 </t>
   </si>
@@ -314,9 +314,6 @@
     </r>
   </si>
   <si>
-    <t>CGEB-IMR (c/o Dr. André Comeau)</t>
-  </si>
-  <si>
     <t>Dept. of Pharmacology, local 5-D</t>
   </si>
   <si>
@@ -363,9 +360,6 @@
   </si>
   <si>
     <t>Quality:</t>
-  </si>
-  <si>
-    <t>10 µL of each sample</t>
   </si>
   <si>
     <t>"clean" DNA coming from commercial kit or proven manual method; absolutely clean spec ratios not required as PCR is relatively robust, but inhibitors must be removed</t>
@@ -405,30 +399,6 @@
   </si>
   <si>
     <t>- purified final library at &gt;10 ng/µL in at least 10 µL; we re-quantify incoming libraries (not oligos below) using Qubit</t>
-  </si>
-  <si>
-    <r>
-      <t>&gt;0.2 ng/µL (preferrably &gt;1 ng/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>µ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>L); we re-quantify incoming DNAs using Qubit or Quant-iT</t>
-    </r>
   </si>
   <si>
     <r>
@@ -1050,6 +1020,9 @@
     <t>For m(meta)transcriptome sequencing (NextSeq):</t>
   </si>
   <si>
+    <t>Coming soon!</t>
+  </si>
+  <si>
     <t>Amount:</t>
   </si>
   <si>
@@ -1089,6 +1062,9 @@
   </si>
   <si>
     <t xml:space="preserve"> MiSeq - ~0.9 million PE 300+300 bp reads = 540 Mb/genome</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PacBio - long-reads of variable size = ~2.0 Gb/genome</t>
   </si>
   <si>
     <t xml:space="preserve"> NextSeq - ~4 million PE 150+150 bp reads = 1.2 Gb/genome</t>
@@ -1145,13 +1121,34 @@
     <t>(separate PCRs</t>
   </si>
   <si>
-    <t xml:space="preserve"> PacBio - ~2.0 Gb/Bact. Genome or ~12 Gb/cell for Euks</t>
-  </si>
-  <si>
-    <t>For Iso-Seq transcriptome sequencing (PacBio):</t>
-  </si>
-  <si>
-    <t>Inquire!</t>
+    <r>
+      <t>&gt;1 ng/µL (preferrably &gt;10 ng/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>µ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>L); we re-quantify incoming DNAs using Qubit or Quant-iT</t>
+    </r>
+  </si>
+  <si>
+    <t>10 µL of each sample (15-20 uL preferred)</t>
+  </si>
+  <si>
+    <t>IMR (c/o Dr. André Comeau)</t>
   </si>
 </sst>
 </file>
@@ -1984,7 +1981,7 @@
     <xf numFmtId="0" fontId="0" fillId="30" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2427,7 +2424,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2442,13 +2441,13 @@
     </row>
     <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" s="14"/>
     </row>
     <row r="3" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B3" s="14"/>
     </row>
@@ -2467,19 +2466,19 @@
     <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
       <c r="B6" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="75" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="32" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -2489,7 +2488,7 @@
     </row>
     <row r="10" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -2514,37 +2513,37 @@
     </row>
     <row r="15" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B16" s="14" t="s">
-        <v>59</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B17" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B18" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B19" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B20" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B21" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2554,10 +2553,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2569,7 +2568,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
@@ -2577,7 +2576,7 @@
     </row>
     <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="82" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B3" s="82"/>
       <c r="C3" s="82"/>
@@ -2585,28 +2584,28 @@
     <row r="4" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="14"/>
       <c r="B4" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="14"/>
       <c r="B5" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="20"/>
       <c r="B6" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="16" t="s">
         <v>75</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>77</v>
       </c>
       <c r="G6" s="16"/>
     </row>
@@ -2616,7 +2615,7 @@
     </row>
     <row r="8" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="83" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B8" s="83"/>
       <c r="C8" s="83"/>
@@ -2624,46 +2623,46 @@
     <row r="9" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="87" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C9" s="87"/>
     </row>
     <row r="10" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="B10" s="88" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C10" s="88"/>
     </row>
     <row r="12" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="86" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B12" s="86"/>
       <c r="C12" s="86"/>
     </row>
     <row r="13" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B13" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>83</v>
+        <v>72</v>
+      </c>
+      <c r="C13" s="81" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B14" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="C14" s="81" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B15" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C15" s="77" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
@@ -2671,33 +2670,33 @@
     </row>
     <row r="17" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="86" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B17" s="86"/>
       <c r="C17" s="86"/>
     </row>
     <row r="18" spans="1:3" s="78" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B18" s="77" t="s">
+        <v>137</v>
+      </c>
+      <c r="C18" s="77" t="s">
         <v>139</v>
-      </c>
-      <c r="C18" s="77" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="78" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B19" s="77" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C19" s="77" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="78" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B20" s="77" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C20" s="77" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
@@ -2705,33 +2704,33 @@
     </row>
     <row r="22" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="84" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B22" s="84"/>
       <c r="C22" s="84"/>
     </row>
     <row r="23" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B23" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="C23" s="22" t="s">
-        <v>83</v>
+        <v>72</v>
+      </c>
+      <c r="C23" s="81" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B24" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="C24" s="81" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B25" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C25" s="77" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
@@ -2739,33 +2738,18 @@
     </row>
     <row r="27" spans="1:3" s="78" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="85" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B27" s="85"/>
       <c r="C27" s="85"/>
     </row>
     <row r="28" spans="1:3" s="78" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B28" s="21" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="85" t="s">
-        <v>156</v>
-      </c>
-      <c r="B30" s="85"/>
-      <c r="C30" s="85"/>
-    </row>
-    <row r="31" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="81"/>
-      <c r="B31" s="21" t="s">
-        <v>157</v>
-      </c>
-      <c r="C31" s="81"/>
+        <v>136</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A30:C30"/>
+  <mergeCells count="8">
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="A22:C22"/>
@@ -2797,7 +2781,7 @@
   <sheetData>
     <row r="1" spans="1:32" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="95" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B1" s="95"/>
       <c r="C1" s="95"/>
@@ -2992,7 +2976,7 @@
     <row r="8" spans="1:32" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="33"/>
       <c r="B8" s="33" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C8" s="106"/>
       <c r="D8" s="107"/>
@@ -3099,7 +3083,7 @@
       <c r="C11" s="63"/>
       <c r="D11" s="63"/>
       <c r="E11" s="75" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F11" s="63"/>
       <c r="G11" s="63"/>
@@ -3133,14 +3117,14 @@
       <c r="A12" s="9"/>
       <c r="B12" s="61"/>
       <c r="D12" s="9" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E12" s="23"/>
       <c r="F12" s="11" t="s">
         <v>40</v>
       </c>
       <c r="I12" s="112" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J12" s="112"/>
       <c r="K12" s="113"/>
@@ -3239,7 +3223,7 @@
       <c r="D15" s="29"/>
       <c r="E15" s="40"/>
       <c r="F15" s="11" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G15" s="12"/>
       <c r="I15" s="112"/>
@@ -3303,7 +3287,7 @@
       <c r="A17" s="33"/>
       <c r="B17" s="60"/>
       <c r="D17" s="33" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E17" s="42"/>
       <c r="F17" s="11" t="s">
@@ -3370,7 +3354,7 @@
       <c r="A19" s="33"/>
       <c r="B19" s="60"/>
       <c r="D19" s="33" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E19" s="43"/>
       <c r="F19" s="11" t="s">
@@ -3378,30 +3362,30 @@
       </c>
       <c r="G19" s="12"/>
       <c r="J19" s="47" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K19" s="48"/>
       <c r="L19" s="11" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="M19" s="35"/>
       <c r="N19" s="51"/>
       <c r="O19" s="11" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="P19" s="35"/>
       <c r="Q19" s="52"/>
       <c r="R19" s="11" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="T19" s="56"/>
       <c r="U19" s="11" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="V19" s="35"/>
       <c r="W19" s="58"/>
       <c r="X19" s="11" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="Y19" s="67"/>
       <c r="Z19" s="35"/>
@@ -3420,27 +3404,27 @@
       <c r="F20" s="11"/>
       <c r="G20" s="12"/>
       <c r="J20" s="79" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K20" s="49"/>
       <c r="L20" s="11" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="M20" s="35"/>
       <c r="N20" s="55"/>
       <c r="O20" s="11" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="P20" s="35"/>
       <c r="Q20" s="53"/>
       <c r="R20" s="11" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S20" s="35"/>
       <c r="V20" s="35"/>
       <c r="W20" s="59"/>
       <c r="X20" s="11" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="Y20" s="67"/>
       <c r="Z20" s="35"/>
@@ -3455,30 +3439,30 @@
       <c r="A21" s="33"/>
       <c r="B21" s="60"/>
       <c r="D21" s="33" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E21" s="46"/>
       <c r="F21" s="11" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G21" s="12"/>
       <c r="J21" s="79" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K21" s="50"/>
       <c r="L21" s="11" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M21" s="35"/>
       <c r="P21" s="35"/>
       <c r="Q21" s="54"/>
       <c r="R21" s="11" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="S21" s="35"/>
       <c r="T21" s="57"/>
       <c r="U21" s="11" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="V21" s="35"/>
       <c r="W21" s="35"/>
@@ -3554,7 +3538,7 @@
       </c>
       <c r="B24" s="93"/>
       <c r="C24" s="96" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D24" s="97"/>
       <c r="E24" s="97"/>
@@ -3585,7 +3569,7 @@
       <c r="A25" s="13"/>
       <c r="B25" s="13"/>
       <c r="C25" s="99" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D25" s="100"/>
       <c r="E25" s="100"/>
@@ -3616,7 +3600,7 @@
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="99" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D26" s="100"/>
       <c r="E26" s="100"/>
@@ -3647,7 +3631,7 @@
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="102" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D27" s="103"/>
       <c r="E27" s="103"/>
@@ -4128,10 +4112,10 @@
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
       <c r="M40" s="36" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="AA40" s="36" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="1:27" x14ac:dyDescent="0.25">
@@ -4503,10 +4487,10 @@
     </row>
     <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="M52" s="36" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="AA52" s="36" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:27" x14ac:dyDescent="0.25">
@@ -5369,7 +5353,7 @@
   <sheetData>
     <row r="1" spans="1:32" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="95" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B1" s="95"/>
       <c r="C1" s="95"/>
@@ -5564,7 +5548,7 @@
     <row r="8" spans="1:32" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="33"/>
       <c r="B8" s="33" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C8" s="106"/>
       <c r="D8" s="107"/>
@@ -5663,7 +5647,7 @@
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="C11" s="13" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D11" s="90"/>
       <c r="E11" s="91"/>
@@ -5720,11 +5704,11 @@
       <c r="A13" s="13"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D13" s="24"/>
       <c r="H13" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I13" s="90"/>
       <c r="J13" s="92"/>
@@ -5774,11 +5758,11 @@
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="C15" s="13" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D15" s="24"/>
       <c r="H15" s="13" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I15" s="90"/>
       <c r="J15" s="92"/>
@@ -5787,11 +5771,11 @@
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C17" s="13" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D17" s="24"/>
       <c r="H17" s="13" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I17" s="90"/>
       <c r="J17" s="92"/>
@@ -5830,7 +5814,7 @@
   <dimension ref="A1:AC26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="M3" sqref="M3:X13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5840,7 +5824,7 @@
   <sheetData>
     <row r="1" spans="1:29" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="95" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B1" s="95"/>
       <c r="C1" s="95"/>
@@ -6015,7 +5999,7 @@
     <row r="8" spans="1:29" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="33"/>
       <c r="B8" s="33" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C8" s="106"/>
       <c r="D8" s="107"/>
@@ -6105,11 +6089,11 @@
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="D11" s="13" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E11" s="26"/>
       <c r="F11" s="11" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="M11" s="94"/>
       <c r="N11" s="94"/>
@@ -6135,7 +6119,7 @@
       <c r="D12" s="13"/>
       <c r="E12" s="80"/>
       <c r="F12" s="11" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="M12" s="94"/>
       <c r="N12" s="94"/>
@@ -6162,7 +6146,7 @@
       <c r="D13" s="11"/>
       <c r="E13" s="25"/>
       <c r="F13" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
@@ -6208,7 +6192,7 @@
       </c>
       <c r="B15" s="93"/>
       <c r="C15" s="96" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D15" s="97"/>
       <c r="E15" s="97"/>
@@ -6236,7 +6220,7 @@
       <c r="A16" s="13"/>
       <c r="B16" s="13"/>
       <c r="C16" s="99" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D16" s="100"/>
       <c r="E16" s="100"/>
@@ -6264,7 +6248,7 @@
       <c r="A17" s="13"/>
       <c r="B17" s="13"/>
       <c r="C17" s="102" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D17" s="103"/>
       <c r="E17" s="103"/>
@@ -6290,39 +6274,39 @@
     </row>
     <row r="19" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="27" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C19" s="118" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D19" s="118"/>
       <c r="E19" s="118"/>
       <c r="F19" s="118"/>
       <c r="G19" s="118" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H19" s="118"/>
       <c r="I19" s="118" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="J19" s="118"/>
       <c r="K19" s="27" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="L19" s="118" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="M19" s="118"/>
       <c r="N19" s="118" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="O19" s="118"/>
       <c r="P19" s="118" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q19" s="118"/>
       <c r="R19" s="115" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="S19" s="115"/>
       <c r="T19" s="115"/>
@@ -6620,7 +6604,7 @@
   <sheetData>
     <row r="1" spans="1:32" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="95" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B1" s="95"/>
       <c r="C1" s="95"/>
@@ -6815,7 +6799,7 @@
     <row r="8" spans="1:32" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="33"/>
       <c r="B8" s="33" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C8" s="106"/>
       <c r="D8" s="107"/>
@@ -6914,11 +6898,11 @@
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="D11" s="13" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E11" s="26"/>
       <c r="F11" s="11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M11" s="94"/>
       <c r="N11" s="94"/>
@@ -6947,7 +6931,7 @@
       <c r="D12" s="13"/>
       <c r="E12" s="44"/>
       <c r="F12" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="M12" s="94"/>
       <c r="N12" s="94"/>
@@ -6977,7 +6961,7 @@
       <c r="D13" s="11"/>
       <c r="E13" s="45"/>
       <c r="F13" s="11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
@@ -7010,7 +6994,7 @@
       <c r="D14" s="11"/>
       <c r="E14" s="42"/>
       <c r="F14" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
@@ -7046,7 +7030,7 @@
       <c r="D15" s="11"/>
       <c r="E15" s="37"/>
       <c r="F15" s="11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
@@ -7102,7 +7086,7 @@
       </c>
       <c r="B17" s="93"/>
       <c r="C17" s="96" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D17" s="97"/>
       <c r="E17" s="97"/>
@@ -7133,7 +7117,7 @@
       <c r="A18" s="13"/>
       <c r="B18" s="13"/>
       <c r="C18" s="99" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D18" s="100"/>
       <c r="E18" s="100"/>
@@ -7164,7 +7148,7 @@
       <c r="A19" s="13"/>
       <c r="B19" s="13"/>
       <c r="C19" s="99" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D19" s="100"/>
       <c r="E19" s="100"/>
@@ -7195,7 +7179,7 @@
       <c r="A20" s="13"/>
       <c r="B20" s="13"/>
       <c r="C20" s="102" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D20" s="103"/>
       <c r="E20" s="103"/>
@@ -8051,7 +8035,7 @@
     </row>
     <row r="49" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A49" s="89" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B49" s="89"/>
       <c r="C49" s="89"/>

</xml_diff>